<commit_message>
NOR-15 Update of test files etc
</commit_message>
<xml_diff>
--- a/ModelCatalogueCorePluginTestApp/test/integration/org/modelcatalogue/core/dataimport/excel/nt/uclh/UCLH_nt_rawimport_AriaTest.xlsx
+++ b/ModelCatalogueCorePluginTestApp/test/integration/org/modelcatalogue/core/dataimport/excel/nt/uclh/UCLH_nt_rawimport_AriaTest.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\ModelCataloguePlugin\ModelCatalogueCorePluginTestApp\test\unit\org\modelcatalogue\integration\excel\nt\uclh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\ModelCataloguePlugin\ModelCatalogueCorePluginTestApp\test\integration\org\modelcatalogue\core\dataimport\excel\nt\uclh\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data items" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,12 +29,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Paul</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
   <si>
     <t>L2</t>
   </si>
@@ -94,9 +95,6 @@
     <t>Value Domain / Data Type</t>
   </si>
   <si>
-    <t>Current Paper Document  or system name</t>
-  </si>
-  <si>
     <t>Semantic Matching</t>
   </si>
   <si>
@@ -227,12 +225,72 @@
   </si>
   <si>
     <t>Related To 2</t>
+  </si>
+  <si>
+    <t>Collected from</t>
+  </si>
+  <si>
+    <t>2.1 Essential Sample Metadata</t>
+  </si>
+  <si>
+    <t>2.1.1 Participant Information</t>
+  </si>
+  <si>
+    <t>2.1.1.1 Patient</t>
+  </si>
+  <si>
+    <t>Surname at Birth (12511.3)</t>
+  </si>
+  <si>
+    <t>The participant's surname at birth, if available and different from current surname</t>
+  </si>
+  <si>
+    <t>personFamilyName(atBirth)</t>
+  </si>
+  <si>
+    <t>PERSON FAMILY NAME (ATBIRTH) (CR0140 from Cancer Outcomes and Services Dataset)</t>
+  </si>
+  <si>
+    <t>COSD</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not recorded </t>
+  </si>
+  <si>
+    <t>Demographic form</t>
+  </si>
+  <si>
+    <t>GEL team</t>
+  </si>
+  <si>
+    <t>CR0140: Person Family Name (at Birth)</t>
+  </si>
+  <si>
+    <t>Person Stated Gender (12509.1)</t>
+  </si>
+  <si>
+    <t>The participant's current gender</t>
+  </si>
+  <si>
+    <t>1..1</t>
+  </si>
+  <si>
+    <t>personStatedGenderCodeEnumerations 2:Female 1:Male9:Not Specified (Unable to be classified as either male or female)X:Not Known (PERSON STATEDGENDER CODE not recorded)</t>
+  </si>
+  <si>
+    <t>PERSON STATED GENDERCODE (CR3170 from Cancer Outcomes and Services Dataset)</t>
+  </si>
+  <si>
+    <t>CR0090: Person Gender Fode (Current)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -341,7 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -368,12 +426,43 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -426,9 +515,9 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="5"/>
-      <tableStyleElement type="headerRow" dxfId="4"/>
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="9"/>
+      <tableStyleElement type="headerRow" dxfId="8"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -443,6 +532,35 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Data items"/>
+      <sheetName val="docstables"/>
+      <sheetName val="Questions"/>
+      <sheetName val="analysis (2)"/>
+      <sheetName val="Flow"/>
+      <sheetName val="Other tables"/>
+      <sheetName val="Copath"/>
+      <sheetName val="HC"/>
+      <sheetName val="COSD"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -767,20 +885,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:ED8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="7" max="7" width="31.36328125" customWidth="1"/>
+    <col min="8" max="8" width="29.36328125" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" customWidth="1"/>
     <col min="11" max="11" width="20.81640625" customWidth="1"/>
     <col min="20" max="20" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:134" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -812,180 +933,180 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:134" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="B2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="N2" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
       <c r="X2" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:134" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="I3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="X3" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:134" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="L4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
@@ -995,112 +1116,505 @@
         <v>1</v>
       </c>
       <c r="X4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y4" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:134" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="11"/>
+      <c r="H5" s="1"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="13"/>
+    </row>
+    <row r="6" spans="1:134" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="8">
+        <v>12511.3</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="U6" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="17">
+        <v>1</v>
+      </c>
+      <c r="W6" s="17">
+        <v>1</v>
+      </c>
+      <c r="X6" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="16"/>
+      <c r="AI6" s="16"/>
+      <c r="AJ6" s="16"/>
+      <c r="AK6" s="16"/>
+      <c r="AL6" s="16"/>
+      <c r="AM6" s="16"/>
+      <c r="AN6" s="16"/>
+      <c r="AO6" s="16"/>
+      <c r="AP6" s="16"/>
+      <c r="AQ6" s="16"/>
+      <c r="AR6" s="16"/>
+      <c r="AS6" s="16"/>
+      <c r="AT6" s="16"/>
+      <c r="AU6" s="16"/>
+      <c r="AV6" s="16"/>
+      <c r="AW6" s="16"/>
+      <c r="AX6" s="16"/>
+      <c r="AY6" s="16"/>
+      <c r="AZ6" s="16"/>
+      <c r="BA6" s="16"/>
+      <c r="BB6" s="16"/>
+      <c r="BC6" s="16"/>
+      <c r="BD6" s="16"/>
+      <c r="BE6" s="16"/>
+      <c r="BF6" s="16"/>
+      <c r="BG6" s="16"/>
+      <c r="BH6" s="16"/>
+      <c r="BI6" s="16"/>
+      <c r="BJ6" s="16"/>
+      <c r="BK6" s="16"/>
+      <c r="BL6" s="16"/>
+      <c r="BM6" s="16"/>
+      <c r="BN6" s="16"/>
+      <c r="BO6" s="16"/>
+      <c r="BP6" s="16"/>
+      <c r="BQ6" s="16"/>
+      <c r="BR6" s="16"/>
+      <c r="BS6" s="16"/>
+      <c r="BT6" s="16"/>
+      <c r="BU6" s="16"/>
+      <c r="BV6" s="16"/>
+      <c r="BW6" s="16"/>
+      <c r="BX6" s="16"/>
+      <c r="BY6" s="16"/>
+      <c r="BZ6" s="16"/>
+      <c r="CA6" s="16"/>
+      <c r="CB6" s="16"/>
+      <c r="CC6" s="16"/>
+      <c r="CD6" s="16"/>
+      <c r="CE6" s="16"/>
+      <c r="CF6" s="16"/>
+      <c r="CG6" s="16"/>
+      <c r="CH6" s="16"/>
+      <c r="CI6" s="16"/>
+      <c r="CJ6" s="16"/>
+      <c r="CK6" s="16"/>
+      <c r="CL6" s="16"/>
+      <c r="CM6" s="16"/>
+      <c r="CN6" s="16"/>
+      <c r="CO6" s="16"/>
+      <c r="CP6" s="16"/>
+      <c r="CQ6" s="16"/>
+      <c r="CR6" s="16"/>
+      <c r="CS6" s="16"/>
+      <c r="CT6" s="16"/>
+      <c r="CU6" s="16"/>
+      <c r="CV6" s="16"/>
+      <c r="CW6" s="16"/>
+      <c r="CX6" s="16"/>
+      <c r="CY6" s="16"/>
+      <c r="CZ6" s="16"/>
+      <c r="DA6" s="16"/>
+      <c r="DB6" s="16"/>
+      <c r="DC6" s="16"/>
+      <c r="DD6" s="16"/>
+      <c r="DE6" s="16"/>
+      <c r="DF6" s="16"/>
+      <c r="DG6" s="16"/>
+      <c r="DH6" s="16"/>
+      <c r="DI6" s="16"/>
+      <c r="DJ6" s="16"/>
+      <c r="DK6" s="16"/>
+      <c r="DL6" s="16"/>
+      <c r="DM6" s="16"/>
+      <c r="DN6" s="16"/>
+      <c r="DO6" s="16"/>
+      <c r="DP6" s="16"/>
+      <c r="DQ6" s="16"/>
+      <c r="DR6" s="16"/>
+      <c r="DS6" s="16"/>
+      <c r="DT6" s="16"/>
+      <c r="DU6" s="16"/>
+      <c r="DV6" s="16"/>
+      <c r="DW6" s="16"/>
+      <c r="DX6" s="16"/>
+      <c r="DY6" s="16"/>
+      <c r="DZ6" s="16"/>
+      <c r="EA6" s="16"/>
+      <c r="EB6" s="16"/>
+      <c r="EC6" s="16"/>
+      <c r="ED6" s="16"/>
+    </row>
+    <row r="7" spans="1:134" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="8">
+        <v>12509.1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="Y4" s="13" t="s">
-        <v>41</v>
-      </c>
+      <c r="O7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="U7" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="17">
+        <v>1</v>
+      </c>
+      <c r="W7" s="17">
+        <v>1</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
+      <c r="AF7" s="16"/>
+      <c r="AG7" s="16"/>
+      <c r="AH7" s="16"/>
+      <c r="AI7" s="16"/>
+      <c r="AJ7" s="16"/>
+      <c r="AK7" s="16"/>
+      <c r="AL7" s="16"/>
+      <c r="AM7" s="16"/>
+      <c r="AN7" s="16"/>
+      <c r="AO7" s="16"/>
+      <c r="AP7" s="16"/>
+      <c r="AQ7" s="16"/>
+      <c r="AR7" s="16"/>
+      <c r="AS7" s="16"/>
+      <c r="AT7" s="16"/>
+      <c r="AU7" s="16"/>
+      <c r="AV7" s="16"/>
+      <c r="AW7" s="16"/>
+      <c r="AX7" s="16"/>
+      <c r="AY7" s="16"/>
+      <c r="AZ7" s="16"/>
+      <c r="BA7" s="16"/>
+      <c r="BB7" s="16"/>
+      <c r="BC7" s="16"/>
+      <c r="BD7" s="16"/>
+      <c r="BE7" s="16"/>
+      <c r="BF7" s="16"/>
+      <c r="BG7" s="16"/>
+      <c r="BH7" s="16"/>
+      <c r="BI7" s="16"/>
+      <c r="BJ7" s="16"/>
+      <c r="BK7" s="16"/>
+      <c r="BL7" s="16"/>
+      <c r="BM7" s="16"/>
+      <c r="BN7" s="16"/>
+      <c r="BO7" s="16"/>
+      <c r="BP7" s="16"/>
+      <c r="BQ7" s="16"/>
+      <c r="BR7" s="16"/>
+      <c r="BS7" s="16"/>
+      <c r="BT7" s="16"/>
+      <c r="BU7" s="16"/>
+      <c r="BV7" s="16"/>
+      <c r="BW7" s="16"/>
+      <c r="BX7" s="16"/>
+      <c r="BY7" s="16"/>
+      <c r="BZ7" s="16"/>
+      <c r="CA7" s="16"/>
+      <c r="CB7" s="16"/>
+      <c r="CC7" s="16"/>
+      <c r="CD7" s="16"/>
+      <c r="CE7" s="16"/>
+      <c r="CF7" s="16"/>
+      <c r="CG7" s="16"/>
+      <c r="CH7" s="16"/>
+      <c r="CI7" s="16"/>
+      <c r="CJ7" s="16"/>
+      <c r="CK7" s="16"/>
+      <c r="CL7" s="16"/>
+      <c r="CM7" s="16"/>
+      <c r="CN7" s="16"/>
+      <c r="CO7" s="16"/>
+      <c r="CP7" s="16"/>
+      <c r="CQ7" s="16"/>
+      <c r="CR7" s="16"/>
+      <c r="CS7" s="16"/>
+      <c r="CT7" s="16"/>
+      <c r="CU7" s="16"/>
+      <c r="CV7" s="16"/>
+      <c r="CW7" s="16"/>
+      <c r="CX7" s="16"/>
+      <c r="CY7" s="16"/>
+      <c r="CZ7" s="16"/>
+      <c r="DA7" s="16"/>
+      <c r="DB7" s="16"/>
+      <c r="DC7" s="16"/>
+      <c r="DD7" s="16"/>
+      <c r="DE7" s="16"/>
+      <c r="DF7" s="16"/>
+      <c r="DG7" s="16"/>
+      <c r="DH7" s="16"/>
+      <c r="DI7" s="16"/>
+      <c r="DJ7" s="16"/>
+      <c r="DK7" s="16"/>
+      <c r="DL7" s="16"/>
+      <c r="DM7" s="16"/>
+      <c r="DN7" s="16"/>
+      <c r="DO7" s="16"/>
+      <c r="DP7" s="16"/>
+      <c r="DQ7" s="16"/>
+      <c r="DR7" s="16"/>
+      <c r="DS7" s="16"/>
+      <c r="DT7" s="16"/>
+      <c r="DU7" s="16"/>
+      <c r="DV7" s="16"/>
+      <c r="DW7" s="16"/>
+      <c r="DX7" s="16"/>
+      <c r="DY7" s="16"/>
+      <c r="DZ7" s="16"/>
+      <c r="EA7" s="16"/>
+      <c r="EB7" s="16"/>
+      <c r="EC7" s="16"/>
+      <c r="ED7" s="16"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="8" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B8">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C8">
         <v>3</v>
       </c>
-      <c r="D5">
+      <c r="D8">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E8">
         <v>5</v>
       </c>
-      <c r="F5">
+      <c r="F8">
         <v>6</v>
       </c>
-      <c r="G5">
+      <c r="G8">
         <v>7</v>
       </c>
-      <c r="H5">
+      <c r="H8">
         <v>8</v>
       </c>
-      <c r="I5">
+      <c r="I8">
         <v>9</v>
       </c>
-      <c r="J5">
+      <c r="J8">
         <v>10</v>
       </c>
-      <c r="K5">
+      <c r="K8">
         <v>11</v>
       </c>
-      <c r="L5">
+      <c r="L8">
         <v>12</v>
       </c>
-      <c r="M5">
+      <c r="M8">
         <v>13</v>
       </c>
-      <c r="N5">
+      <c r="N8">
         <v>14</v>
       </c>
-      <c r="O5">
+      <c r="O8">
         <v>15</v>
       </c>
-      <c r="P5">
+      <c r="P8">
         <v>16</v>
       </c>
-      <c r="Q5">
+      <c r="Q8">
         <v>17</v>
       </c>
-      <c r="R5">
+      <c r="R8">
         <v>18</v>
       </c>
-      <c r="S5">
+      <c r="S8">
         <v>19</v>
       </c>
-      <c r="T5">
+      <c r="T8">
         <v>20</v>
       </c>
-      <c r="U5">
+      <c r="U8">
         <v>21</v>
       </c>
-      <c r="V5">
+      <c r="V8">
         <v>22</v>
       </c>
-      <c r="W5">
+      <c r="W8">
         <v>23</v>
       </c>
-      <c r="X5">
+      <c r="X8">
         <v>24</v>
       </c>
-      <c r="Y5">
+      <c r="Y8">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="X1:X4 M1:M4">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="X1:X5 M1:M5">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L4">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="L1:L5">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Not recorded "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X4">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="X2:X5">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Unknown"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="M2:M5">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Unknown"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L6:L7">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Not recorded "</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X6:X7 M6:M7">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X6:X7">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Unknown"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M6:M7">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Unknown"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1:X4 M2:M4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M7 X1:X7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No,Unknown"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1108,12 +1622,18 @@
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'C:\Users\david\Desktop\[UCLH Cancerdatamaster v6.xlsx]docstables'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L4</xm:sqref>
+          <xm:sqref>L2:L5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F8C4D91A-3AFC-4D6F-A4B4-19C2AAC165F5}">
+          <x14:formula1>
+            <xm:f>'C:\Operations\NorthThames\General\rawimportsheets\[uclh_nt_rawimport.xlsx]docstables'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>L6:L7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1122,7 +1642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1133,7 +1653,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>6</v>
@@ -1142,25 +1662,25 @@
         <v>7</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -1168,19 +1688,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>50</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>

</xml_diff>